<commit_message>
mise a jour heure arnaud
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal_Ramirez_Arnaud.xlsx
+++ b/documentation/3_1_Journal_Ramirez_Arnaud.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repoGit\306-G2-ArcadiaBox\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arnaud\306project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3237F3F8-34CA-4672-BB56-C8604E58B8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E970C14C-7B46-46CE-9493-102A6293AD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_RAMIREZ_ARNAUD" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Journal_NOM_PRENOM4!$B:$D,Journal_NOM_PRENOM4!$1:$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal_RAMIREZ_ARNAUD!$B:$D,Journal_RAMIREZ_ARNAUD!$1:$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Journal_NOM_PRENOM4!$A$1:$D$83</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal_RAMIREZ_ARNAUD!$A$1:$D$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal_RAMIREZ_ARNAUD!$A$1:$D$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -166,6 +166,24 @@
   <si>
     <t>J’ai bien aimé pouvoir commencer le projet et être plutôt libre. J’ai une petite frustration car j’ai l’impression d’avoir perdu pas mal de temps sur la documentation d’EmulatorJS. Cependant, je pense que ce sera quand même utilisé par la suite.</t>
   </si>
+  <si>
+    <t>sprint review</t>
+  </si>
+  <si>
+    <t>Sprint Planing</t>
+  </si>
+  <si>
+    <t>Coder la page principale avec la sélections des jeux</t>
+  </si>
+  <si>
+    <t>Déployer les services (base de donné)</t>
+  </si>
+  <si>
+    <t>Création de l'api / Création d'une route pour tester</t>
+  </si>
+  <si>
+    <t>Recherche sur le score</t>
+  </si>
 </sst>
 </file>
 
@@ -479,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -528,6 +546,62 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -564,10 +638,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -576,56 +646,26 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1522,111 +1562,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971094A1-2086-4124-85CF-EAAE0115819F}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1"/>
-    <col min="2" max="3" width="31.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="217" width="9.109375" style="1" customWidth="1"/>
-    <col min="218" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1"/>
+    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="217" width="9.140625" style="1" customWidth="1"/>
+    <col min="218" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="35">
         <v>45996</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="25" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="25" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8">
         <v>1.8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1638,68 +1678,68 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="27" t="s">
+    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
         <v>46003</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="32"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="25" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="25" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="26"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="8">
         <v>3.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1711,547 +1751,516 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="27" t="s">
+    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14">
+        <v>46009</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="9">
-        <f>SUM(D20:D24)</f>
+      <c r="D27" s="9">
+        <f>SUM(D20:D26)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14">
+        <v>46010</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="9">
+        <f>SUM(D29:D33)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="16"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+    </row>
+    <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="15"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="15"/>
+      <c r="B41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="9">
+        <f>SUM(D36:D40)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="2" t="s">
+    <row r="42" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="16"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+    </row>
+    <row r="43" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="15"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="15"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="15"/>
+      <c r="B48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="9">
-        <f>SUM(D27:D31)</f>
+      <c r="D48" s="9">
+        <f>SUM(D43:D47)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="36"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="2" t="s">
+    <row r="49" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="16"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="15"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="15"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="15"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="15"/>
+      <c r="B55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="9">
-        <f>SUM(D34:D38)</f>
+      <c r="D55" s="9">
+        <f>SUM(D50:D54)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="36"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="8"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="2" t="s">
+    <row r="56" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="16"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="15"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="15"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="15"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="15"/>
+      <c r="B62" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="9">
-        <f>SUM(D41:D45)</f>
+      <c r="D62" s="9">
+        <f>SUM(D57:D61)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="36"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="2" t="s">
+    <row r="63" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="16"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="23"/>
+    </row>
+    <row r="64" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="15"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="15"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="15"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="15"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="15"/>
+      <c r="B69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="9">
-        <f>SUM(D48:D52)</f>
+      <c r="D69" s="9">
+        <f>SUM(D64:D68)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="36"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="8"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="8"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="8"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="2" t="s">
+    <row r="70" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="15"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="26"/>
+    </row>
+    <row r="71" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="7"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="15"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="8"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="15"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="15"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="15"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="15"/>
+      <c r="B76" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="9">
-        <f>SUM(D55:D59)</f>
+      <c r="D76" s="9">
+        <f>SUM(D71:D75)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="7"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="8"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="8"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="22"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="8"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="22"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="8"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
-      <c r="B67" s="2" t="s">
+    <row r="77" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="16"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="23"/>
+    </row>
+    <row r="78" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="14"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="15"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="15"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="15"/>
+      <c r="B83" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D67" s="9">
-        <f>SUM(D62:D66)</f>
+      <c r="D83" s="9">
+        <f>SUM(D78:D82)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="29"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="22"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="8"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="22"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="8"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="22"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="22"/>
-      <c r="B74" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="9">
-        <f>SUM(D69:D73)</f>
+    <row r="84" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="16"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="23"/>
+    </row>
+    <row r="85" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="11"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="12">
+        <f>D11+D18+D27+D34+D41+D48+D55+D62+D69+D76+D83</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="33"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="36"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
-      <c r="B76" s="31"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="7"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="22"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="8"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="22"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="8"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="22"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="8"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="22"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="8"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="22"/>
-      <c r="B81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D81" s="9">
-        <f>SUM(D76:D80)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="33"/>
-      <c r="B82" s="34"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="36"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" s="12">
-        <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
+  <mergeCells count="84">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -2263,6 +2272,79 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="A64:A70"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="A71:A77"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B84:D84"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="47" priority="23" operator="containsText" text="Terminé">
@@ -2280,7 +2362,7 @@
       <formula>NOT(ISERROR(SEARCH("En cours",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20:D25">
+  <conditionalFormatting sqref="D20:D27">
     <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D20)))</formula>
     </cfRule>
@@ -2288,76 +2370,76 @@
       <formula>NOT(ISERROR(SEARCH("En cours",D20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27:D32">
+  <conditionalFormatting sqref="D29:D34">
     <cfRule type="containsText" dxfId="41" priority="19" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D39">
+  <conditionalFormatting sqref="D36:D41">
     <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D34)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D36)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D34)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D46">
+  <conditionalFormatting sqref="D43:D48">
     <cfRule type="containsText" dxfId="37" priority="9" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D43)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="10" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D43)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D53">
+  <conditionalFormatting sqref="D50:D55">
     <cfRule type="containsText" dxfId="35" priority="7" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D50)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55:D60">
+  <conditionalFormatting sqref="D57:D62">
     <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D57)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62:D67">
+  <conditionalFormatting sqref="D64:D69">
     <cfRule type="containsText" dxfId="31" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D64)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69:D74">
+  <conditionalFormatting sqref="D71:D76">
     <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D71)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D76:D81">
+  <conditionalFormatting sqref="D78:D83">
     <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D76)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D78)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="12" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D76)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D78)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D83">
+  <conditionalFormatting sqref="D85">
     <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D85)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -2369,8 +2451,8 @@
     <oddFooter>&amp;L&amp;8&amp;F&amp;R&amp;8Page &amp;P/&amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="47" max="16383" man="1"/>
-    <brk id="83" max="3" man="1"/>
+    <brk id="49" max="16383" man="1"/>
+    <brk id="85" max="3" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
@@ -2386,85 +2468,85 @@
       <selection pane="bottomLeft" activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1"/>
-    <col min="2" max="3" width="31.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="217" width="9.109375" style="1" customWidth="1"/>
-    <col min="218" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1"/>
+    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="217" width="9.140625" style="1" customWidth="1"/>
+    <col min="218" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2476,44 +2558,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
+    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2525,44 +2607,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
+    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
@@ -2574,44 +2656,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
+    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -2623,44 +2705,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="36"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
+    <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="16"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="14"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="26"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="15"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="26"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2672,44 +2754,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="36"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="32"/>
+    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="16"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="26"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="15"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="26"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="15"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="20"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="26"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="15"/>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -2721,44 +2803,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="36"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="32"/>
+    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="16"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="26"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="15"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="15"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="26"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="15"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="26"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>8</v>
       </c>
@@ -2770,44 +2852,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="36"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="32"/>
+    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="16"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="26"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="15"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="20"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="26"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="15"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="20"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="26"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="20"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="26"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="15"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="20"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="15"/>
       <c r="B60" s="2" t="s">
         <v>8</v>
       </c>
@@ -2819,44 +2901,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="32"/>
+    <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="16"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="23"/>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="26"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="15"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="20"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="26"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="15"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="22"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="26"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="15"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="22"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="26"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="15"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
@@ -2868,44 +2950,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="29"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="32"/>
+    <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="15"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="26"/>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="14"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="18"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="22"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="26"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="15"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="26"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="15"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="22"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="26"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="15"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="22"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="26"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="15"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="20"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="22"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="15"/>
       <c r="B74" s="2" t="s">
         <v>8</v>
       </c>
@@ -2917,44 +2999,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="33"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="36"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
-      <c r="B76" s="31"/>
-      <c r="C76" s="32"/>
+    <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="16"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="23"/>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="18"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="22"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="26"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="15"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="20"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="22"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="26"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="15"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="22"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="26"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="20"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="22"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="26"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="22"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="15"/>
       <c r="B81" s="2" t="s">
         <v>8</v>
       </c>
@@ -2966,13 +3048,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="33"/>
-      <c r="B82" s="34"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="36"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="16"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="23"/>
+    </row>
+    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
       <c r="B83" s="10"/>
       <c r="C83" s="3" t="s">
@@ -2983,87 +3065,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="37" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -3075,6 +3086,77 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -3198,6 +3280,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -3410,17 +3503,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
@@ -3430,6 +3512,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
+    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3446,17 +3541,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>